<commit_message>
Inbetween commit. The script /home/matthias/1_local_code/mf-2/projectmf/data/nutrient_profile/make_nutrient_profile_from_dri_excel_file.py has been finished. It is clunky, but it is not a central part of the application so that is okay. It works, meaning it produces the correct JSON file: nutrient_profiles_from_national_institute_of_health.json.
</commit_message>
<xml_diff>
--- a/projectmf/data/daily_recommended_intake.xlsx
+++ b/projectmf/data/daily_recommended_intake.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="dri_elements" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="211">
   <si>
     <t xml:space="preserve">Life Stage
 Group</t>
@@ -606,6 +606,93 @@
   </si>
   <si>
     <t xml:space="preserve">Vanadium (mg/d)d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life Stage Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromium (μg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copper (μg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluoride (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iodine (μg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnesium (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manganese (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molybdenum (μg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phosphorus (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selenium (μg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zinc (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potassium (g/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodium (g/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chloride (g/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin C (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin D (μg/d)b,c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin K (μg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiamin (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riboflavin (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin B6 (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin B12 (μg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pantothenic Acid (mg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biotin (μg/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbohydrate (g/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Fiber (g/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fat (g/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linoleic Acid (g/d)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">α-Linolenic Acid (g/d)</t>
   </si>
 </sst>
 </file>
@@ -709,7 +796,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="Q1:AI29 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1916,7 +2003,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="Q1:AI29 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3054,7 +3141,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="Q1:AI29 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3709,7 +3796,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="Q1:AI29 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4916,7 +5003,7 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="Q1:AI29 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6398,102 +6485,139 @@
   </sheetPr>
   <dimension ref="A1:AK29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE1" activeCellId="0" sqref="Q1:AI29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="21.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="16.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="17.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="8.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="19.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="12.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="38" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>182</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
+      <c r="C1" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>196</v>
       </c>
       <c r="Q1" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>86</v>
+      <c r="R1" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>198</v>
       </c>
       <c r="T1" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>90</v>
+      <c r="U1" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>201</v>
       </c>
       <c r="X1" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>92</v>
+      <c r="Y1" s="0" t="s">
+        <v>202</v>
       </c>
       <c r="Z1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>96</v>
+      <c r="AA1" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>205</v>
       </c>
       <c r="AD1" s="0" t="s">
         <v>97</v>
@@ -6501,20 +6625,20 @@
       <c r="AE1" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>134</v>
+      <c r="AF1" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="AH1" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="AI1" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>210</v>
       </c>
       <c r="AK1" s="0" t="s">
         <v>135</v>
@@ -9054,8 +9178,8 @@
   </sheetPr>
   <dimension ref="A1:AI29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1:AI29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
It is now possible to add the nutrient profiles from the national institute of health to the measuredfood application. The relevant scripts are make_nutrient_profile_from_dri_excel_file.py and add_nutrientprofile_selenium_national_institute_of_health.py, and they both work.
</commit_message>
<xml_diff>
--- a/projectmf/data/daily_recommended_intake.xlsx
+++ b/projectmf/data/daily_recommended_intake.xlsx
@@ -6486,7 +6486,7 @@
   <dimension ref="A1:AK29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7791,7 +7791,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Commit before significant manipulation: The max tolerable upper intakes of the nutrient profiles are integrated as well.
</commit_message>
<xml_diff>
--- a/projectmf/data/daily_recommended_intake.xlsx
+++ b/projectmf/data/daily_recommended_intake.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dri_elements" sheetId="1" state="visible" r:id="rId2"/>
@@ -3140,8 +3140,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6485,7 +6485,7 @@
   </sheetPr>
   <dimension ref="A1:AK29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>

</xml_diff>